<commit_message>
OW-425 changed the indexes name missing in clarus
</commit_message>
<xml_diff>
--- a/valuation-app/src/test/resources/excel/P45-P46.xlsx
+++ b/valuation-app/src/test/resources/excel/P45-P46.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="IRS-Cleared" sheetId="1" state="visible" r:id="rId2"/>
@@ -677,7 +677,7 @@
     <t xml:space="preserve">4.45</t>
   </si>
   <si>
-    <t xml:space="preserve">NOK-NIBOR-NIBR</t>
+    <t xml:space="preserve">NOK-NIBOR-OIBOR</t>
   </si>
   <si>
     <t xml:space="preserve">500021</t>
@@ -803,7 +803,7 @@
     <t xml:space="preserve">SGSI</t>
   </si>
   <si>
-    <t xml:space="preserve">SGD-SOR-Reuters</t>
+    <t xml:space="preserve">SGD-SOR-VWAP</t>
   </si>
   <si>
     <t xml:space="preserve">500026</t>
@@ -1229,65 +1229,64 @@
   </sheetPr>
   <dimension ref="A1:BE51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F49" activeCellId="0" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="43" min="42" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="34.4234693877551"/>
-    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="50" min="49" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="56" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="31.0459183673469"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="31.0459183673469"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="43" min="42" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="50" min="49" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="51" min="51" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="52" min="52" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="53" min="53" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="54" min="54" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="55" min="55" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="56" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9570,56 +9569,56 @@
   </sheetPr>
   <dimension ref="A1:AR51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AI1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V19" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AC41" activeCellId="0" sqref="AC41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="45" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="45" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>